<commit_message>
Update rdf files based on Voorstel metainformatie catalogus-Arjen.xlsx
</commit_message>
<xml_diff>
--- a/sessies/metadata/Voorstel metainformatie Catalogus-Arjen.xlsx
+++ b/sessies/metadata/Voorstel metainformatie Catalogus-Arjen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hetkadaster-my.sharepoint.com/personal/arjen_santema_kadaster_nl/Documents/Mijn Documenten/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hetkadaster-my.sharepoint.com/personal/jesse_bakker_kadaster_nl/Documents/Documenten/Projects/nederlands-profiel-voor-stelselcatalogi/sessies/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47B116F5-9A33-475B-90FD-5753FD24EED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{47B116F5-9A33-475B-90FD-5753FD24EED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D807ED5B-3D7A-4DD1-9E0D-8766B775C157}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{E116C561-E918-B349-9B9B-ADD36732EA7D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{E116C561-E918-B349-9B9B-ADD36732EA7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Voorstel velden metadata" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="150">
   <si>
     <t>Toelichting</t>
   </si>
@@ -147,10 +147,6 @@
   </si>
   <si>
     <t xml:space="preserve">Een optie is om hier prov:qualifiedAttribution te gebruiken, met bereik https://www.w3.org/TR/prov-o/#Attribution </t>
-  </si>
-  <si>
-    <t>dct:accrualPeriodicity
- https://standaarden.overheid.nl/owms/terms/Frequentie</t>
   </si>
   <si>
     <t>Deze eigenschap verwijst naar de vastgestelde standaard waaraan de data van de beschreven resource voldoet. Hierbij kan worden gedacht aan het model, schema, ontology, view of profiel.</t>
@@ -428,9 +424,6 @@
     <t>Typering</t>
   </si>
   <si>
-    <t>skos:conceptScheme; adms:Asset</t>
-  </si>
-  <si>
     <t>sh:order</t>
   </si>
   <si>
@@ -498,10 +491,20 @@
     <t>type</t>
   </si>
   <si>
-    <t>skos:ConceptScheme</t>
-  </si>
-  <si>
     <t>dcterms:Standard</t>
+  </si>
+  <si>
+    <t>rdf:type</t>
+  </si>
+  <si>
+    <t>skos:conceptScheme, adms:Asset</t>
+  </si>
+  <si>
+    <t>dct:accrualPeriodicity,
+ https://standaarden.overheid.nl/owms/terms/Frequentie</t>
+  </si>
+  <si>
+    <t>skos:Concept</t>
   </si>
 </sst>
 </file>
@@ -635,12 +638,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -679,6 +676,12 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -997,226 +1000,226 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{011F12BD-9210-2748-B977-A34CB11C8463}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8:D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.69921875" customWidth="1"/>
+    <col min="1" max="1" width="21.75" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="13.796875" customWidth="1"/>
-    <col min="4" max="4" width="51.796875" customWidth="1"/>
-    <col min="5" max="5" width="17.296875" customWidth="1"/>
+    <col min="3" max="3" width="13.75" customWidth="1"/>
+    <col min="4" max="4" width="51.75" customWidth="1"/>
+    <col min="5" max="5" width="17.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-    </row>
-    <row r="3" spans="1:5" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+    <row r="1" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+    </row>
+    <row r="3" spans="1:5" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+    </row>
+    <row r="4" spans="1:5" ht="36.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+    </row>
+    <row r="5" spans="1:5" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
         <v>49</v>
-      </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-    </row>
-    <row r="4" spans="1:5" ht="36.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-    </row>
-    <row r="5" spans="1:5" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" t="s">
-        <v>50</v>
       </c>
       <c r="C8" s="7">
         <v>44669</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9" s="7">
         <v>44671</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" t="s">
         <v>71</v>
-      </c>
-      <c r="B10" t="s">
-        <v>72</v>
       </c>
       <c r="C10" s="7">
         <v>44699</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C11" s="7">
         <v>44714</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C12" s="7">
         <v>44721</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C13" s="7"/>
       <c r="D13" s="10"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C14" s="7"/>
       <c r="D14" s="10"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C15" s="7"/>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C16" s="7"/>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C17" s="7"/>
       <c r="D17" s="10"/>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C18" s="7"/>
       <c r="D18" s="10"/>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C19" s="7"/>
       <c r="D19" s="10"/>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D20" s="10"/>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D21" s="10"/>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D22" s="10"/>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D23" s="10"/>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D24" s="10"/>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D25" s="10"/>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D26" s="10"/>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D27" s="10"/>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D28" s="10"/>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D29" s="10"/>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D30" s="10"/>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D31" s="10"/>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D32" s="10"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" s="10"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" s="10"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" s="10"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D36" s="10"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D37" s="10"/>
     </row>
   </sheetData>
@@ -1236,109 +1239,112 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45A42D6-0C39-914F-9BC8-C6AECC16103C}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.3984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.19921875" customWidth="1"/>
-    <col min="4" max="4" width="7.796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.296875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="23.296875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="11.19921875" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.59765625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.59765625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="45.796875" style="4" customWidth="1"/>
-    <col min="11" max="11" width="51.19921875" customWidth="1"/>
-    <col min="12" max="12" width="41.69921875" style="16" customWidth="1"/>
+    <col min="1" max="1" width="16.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.25" customWidth="1"/>
+    <col min="4" max="4" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.25" style="4" customWidth="1"/>
+    <col min="6" max="6" width="52.5" style="4" customWidth="1"/>
+    <col min="7" max="7" width="11.25" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="45.75" style="4" customWidth="1"/>
+    <col min="11" max="11" width="51.25" customWidth="1"/>
+    <col min="12" max="12" width="41.75" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="8" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
-        <v>146</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>111</v>
+    <row r="1" spans="1:12" s="8" customFormat="1" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>110</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D1" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>128</v>
-      </c>
       <c r="J1" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>21</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="109.2" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>124</v>
+        <v>125</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>123</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="G2" s="23">
+        <v>146</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G2" s="21">
         <v>1</v>
       </c>
       <c r="J2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="K2" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="L2" s="16" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="14" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="14" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D3" s="11">
         <v>1</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F3" s="12"/>
-      <c r="G3" s="21">
+      <c r="G3" s="19">
         <v>1</v>
       </c>
       <c r="H3" s="12">
@@ -1351,15 +1357,15 @@
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
     </row>
-    <row r="4" spans="1:12" s="14" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" s="14" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D4" s="11">
         <v>2</v>
@@ -1368,63 +1374,63 @@
         <v>20</v>
       </c>
       <c r="F4" s="13"/>
-      <c r="G4" s="22"/>
+      <c r="G4" s="20"/>
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
       <c r="J4" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:12" s="14" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" s="14" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D5" s="11">
         <v>3</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F5" s="12"/>
-      <c r="G5" s="21"/>
+      <c r="G5" s="19"/>
       <c r="H5" s="12">
         <v>1</v>
       </c>
       <c r="I5" s="12"/>
       <c r="J5" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K5" s="13"/>
       <c r="L5" s="13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="14" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="14" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D6" s="11">
         <v>4</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F6" s="12"/>
-      <c r="G6" s="21">
+      <c r="G6" s="19">
         <v>1</v>
       </c>
       <c r="H6" s="12">
@@ -1432,18 +1438,18 @@
       </c>
       <c r="I6" s="12"/>
       <c r="J6" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L6" s="13" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="14" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="14" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>0</v>
@@ -1458,156 +1464,156 @@
         <v>21</v>
       </c>
       <c r="F7" s="12"/>
-      <c r="G7" s="21"/>
+      <c r="G7" s="19"/>
       <c r="H7" s="12">
         <v>1</v>
       </c>
       <c r="I7" s="12"/>
       <c r="J7" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K7" s="13"/>
       <c r="L7" s="13" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>82</v>
+        <v>128</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>81</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D8" s="6">
         <v>6</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D9" s="11">
         <v>7</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F9" s="12"/>
-      <c r="G9" s="21"/>
+      <c r="G9" s="19"/>
       <c r="H9" s="12">
         <v>1</v>
       </c>
       <c r="I9" s="12"/>
       <c r="J9" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
     </row>
-    <row r="10" spans="1:12" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>64</v>
+        <v>130</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>63</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D10" s="6">
         <v>8</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H10" s="4">
         <v>1</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:12" s="30" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="26" t="s">
+    <row r="11" spans="1:12" s="28" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="24"/>
+      <c r="B11" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="25"/>
+      <c r="E11" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="26"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="26">
-        <v>1</v>
-      </c>
-      <c r="I11" s="26"/>
-      <c r="J11" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="K11" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="L11" s="29"/>
-    </row>
-    <row r="12" spans="1:12" s="30" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>116</v>
-      </c>
-      <c r="C12" s="27" t="s">
+      <c r="F11" s="24"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="24">
+        <v>1</v>
+      </c>
+      <c r="I11" s="24"/>
+      <c r="J11" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="K11" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="L11" s="27"/>
+    </row>
+    <row r="12" spans="1:12" s="28" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="27">
+      <c r="D12" s="25">
         <v>9</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="26"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="26">
-        <v>1</v>
-      </c>
-      <c r="I12" s="26"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="L12" s="29"/>
-    </row>
-    <row r="13" spans="1:12" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="F12" s="24"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="24">
+        <v>1</v>
+      </c>
+      <c r="I12" s="24"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="L12" s="27"/>
+    </row>
+    <row r="13" spans="1:12" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B13" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" s="17" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -1620,26 +1626,26 @@
         <v>15</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="G13" s="23">
+        <v>134</v>
+      </c>
+      <c r="G13" s="21">
         <v>1</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L13" s="16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="93.6" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B14" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="B14" s="17" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -1649,10 +1655,10 @@
         <v>11</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H14" s="4">
         <v>1</v>
@@ -1664,14 +1670,14 @@
         <v>31</v>
       </c>
       <c r="L14" s="16" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B15" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="B15" s="17" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="6" t="s">
@@ -1684,7 +1690,7 @@
         <v>24</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H15" s="4">
         <v>1</v>
@@ -1694,11 +1700,11 @@
       </c>
       <c r="K15" s="5"/>
     </row>
-    <row r="16" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B16" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="B16" s="17" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="6" t="s">
@@ -1708,21 +1714,21 @@
         <v>13</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>32</v>
       </c>
       <c r="K16" s="5"/>
     </row>
-    <row r="17" spans="1:12" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="63" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B17" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="B17" s="17" t="s">
         <v>28</v>
       </c>
       <c r="C17" s="6" t="s">
@@ -1732,10 +1738,10 @@
         <v>14</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H17" s="4">
         <v>1</v>
@@ -1747,14 +1753,14 @@
         <v>36</v>
       </c>
       <c r="L17" s="16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="46.8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B18" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="B18" s="17" t="s">
         <v>29</v>
       </c>
       <c r="C18" s="6" t="s">
@@ -1764,10 +1770,10 @@
         <v>15</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H18" s="4">
         <v>1</v>
@@ -1777,15 +1783,15 @@
       </c>
       <c r="K18" s="5"/>
       <c r="L18" s="16" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>117</v>
+        <v>128</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>116</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>4</v>
@@ -1802,11 +1808,11 @@
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
     </row>
-    <row r="20" spans="1:12" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="63" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B20" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="B20" s="17" t="s">
         <v>14</v>
       </c>
       <c r="C20" s="6" t="s">
@@ -1816,27 +1822,27 @@
         <v>17</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H20" s="4">
         <v>1</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="L20" s="32" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="62.4" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+      <c r="L20" s="30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="63" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>118</v>
+        <v>128</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>117</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>12</v>
@@ -1845,10 +1851,10 @@
         <v>18</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>37</v>
+        <v>148</v>
       </c>
       <c r="F21" s="15"/>
-      <c r="G21" s="24"/>
+      <c r="G21" s="22"/>
       <c r="H21" s="4">
         <v>1</v>
       </c>
@@ -1857,14 +1863,14 @@
       </c>
       <c r="K21" s="5"/>
       <c r="L21" s="16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="46.8" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B22" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="B22" s="17" t="s">
         <v>13</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -1874,21 +1880,21 @@
         <v>19</v>
       </c>
       <c r="E22" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H22" s="4">
+        <v>1</v>
+      </c>
+      <c r="J22" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H22" s="4">
-        <v>1</v>
-      </c>
-      <c r="J22" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="K22" s="5"/>
     </row>
-    <row r="23" spans="1:12" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B23" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="B23" s="17" t="s">
         <v>9</v>
       </c>
       <c r="C23" s="6" t="s">
@@ -1898,30 +1904,30 @@
         <v>20</v>
       </c>
       <c r="E23" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="F23" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="F23" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="G23" s="24"/>
+      <c r="G23" s="22"/>
       <c r="H23" s="4">
         <v>1</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L23" s="16" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="62.4" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="63" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B24" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="B24" s="17" t="s">
         <v>6</v>
       </c>
       <c r="C24" s="6" t="s">
@@ -1930,11 +1936,11 @@
       <c r="D24" s="6">
         <v>21</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="E24" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="F24" s="16" t="s">
         <v>143</v>
-      </c>
-      <c r="F24" s="16" t="s">
-        <v>145</v>
       </c>
       <c r="H24" s="4">
         <v>1</v>
@@ -1943,18 +1949,18 @@
         <v>35</v>
       </c>
       <c r="K24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L24" s="16" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="62.4" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="63" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B25" s="19" t="s">
-        <v>119</v>
+        <v>130</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>118</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>10</v>
@@ -1963,27 +1969,27 @@
         <v>22</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H25" s="4">
         <v>1</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="78" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B26" s="19" t="s">
-        <v>120</v>
+        <v>130</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>119</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>8</v>
@@ -1995,23 +2001,23 @@
         <v>18</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="J26" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="K26" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="K26" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="L26" s="16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B27" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="B27" s="17" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="6" t="s">
@@ -2024,10 +2030,10 @@
         <v>17</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>